<commit_message>
Changed Radius Values, Skidpad Wierd Output
</commit_message>
<xml_diff>
--- a/TrackDetails.xlsx
+++ b/TrackDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="5" r:id="rId1"/>
@@ -376,7 +376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -438,6 +438,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>58</v>
+      </c>
+      <c r="C1">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>58</v>
+      </c>
+      <c r="C2">
+        <v>9.125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -449,10 +486,10 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="C1">
-        <v>16.75</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -460,10 +497,43 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>16.75</v>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -471,12 +541,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,78 +556,10 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>20.3</v>
+        <v>13</v>
       </c>
       <c r="C1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>20.3</v>
-      </c>
-      <c r="C2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>20.3</v>
-      </c>
-      <c r="C3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>20.3</v>
-      </c>
-      <c r="C4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>20.3</v>
-      </c>
-      <c r="C5">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>12</v>
-      </c>
-      <c r="C1">
-        <v>7.25</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Skidpad Wierd Output, Cleanup/Reorder Code
</commit_message>
<xml_diff>
--- a/TrackDetails.xlsx
+++ b/TrackDetails.xlsx
@@ -436,10 +436,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +449,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="C1">
         <v>9.125</v>
@@ -460,9 +460,1263 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="C2">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>0</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>0</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>0</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>0</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>0</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>0</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>0</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>0</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>0</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>0</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>0</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>0</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>0</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>0</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>0</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>0</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>0</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>0</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>0</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>0</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>0</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>0</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>0</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>0</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>0</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>0</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>0</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>0</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>0</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>0</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>0</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>0</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>0</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>0</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>0</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>0</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>0</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="C112">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>0</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="C113">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>0</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>0</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="C115">
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>0</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+      <c r="C116">
         <v>9.125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tested with 5mm version works. 1mm program unable to run.
</commit_message>
<xml_diff>
--- a/TrackDetails.xlsx
+++ b/TrackDetails.xlsx
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,14 +400,14 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>3</v>
       </c>
@@ -429,12 +429,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>7</v>
       </c>
@@ -452,9 +452,9 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -481,9 +481,9 @@
       <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -497,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -511,7 +511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -525,7 +525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -539,7 +539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -567,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -581,7 +581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -595,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -637,7 +637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -651,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -665,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -679,7 +679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -721,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -749,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -763,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -777,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -791,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -805,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -819,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -833,7 +833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -861,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -875,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -903,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -917,7 +917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0</v>
       </c>
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -987,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0</v>
       </c>
@@ -2120,9 +2120,9 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2205,9 +2205,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -2228,15 +2228,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2320,39 +2320,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7">
         <v>32</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>10</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
         <v>35</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>999999</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>